<commit_message>
results 0.22 - added human scored documents
</commit_message>
<xml_diff>
--- a/results/scored/HCC_hpo.xlsx
+++ b/results/scored/HCC_hpo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/PhD/Projects/LLM PICO/validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/pico-parser-llm/results/scored/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220FADDC-7CD3-0C46-A380-792AF3E92F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659D5747-6451-6440-AE6F-2D121B6E432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34640" windowHeight="28300" firstSheet="1" activeTab="7" xr2:uid="{94ED0F72-83BA-0D42-BD77-66A26D61B195}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{94ED0F72-83BA-0D42-BD77-66A26D61B195}"/>
   </bookViews>
   <sheets>
     <sheet name="HCC_PC_base" sheetId="13" r:id="rId1"/>
@@ -1815,13 +1815,13 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2215,8 +2215,8 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25" defaultRowHeight="40" customHeight="1"/>
@@ -3005,7 +3005,7 @@
       <c r="B3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3017,7 +3017,7 @@
       <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="32"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -3029,7 +3029,7 @@
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="32"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3041,7 +3041,7 @@
       <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="32"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -3053,7 +3053,7 @@
       <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="32"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3065,7 +3065,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -3077,7 +3077,7 @@
       <c r="B9" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -3089,7 +3089,7 @@
       <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -3101,7 +3101,7 @@
       <c r="B11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="65"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -3113,7 +3113,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="65"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -3149,7 +3149,7 @@
       <c r="B15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="65"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -3161,7 +3161,7 @@
       <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="65"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -3173,7 +3173,7 @@
       <c r="B17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="65"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3185,7 +3185,7 @@
       <c r="B18" s="45">
         <v>0.5</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="65"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -3221,7 +3221,7 @@
       <c r="B21" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -3233,7 +3233,7 @@
       <c r="B22" s="45">
         <v>1</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3269,7 +3269,7 @@
       <c r="B25" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="68"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="12"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -3281,7 +3281,7 @@
       <c r="B26" s="45">
         <v>1</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -3293,7 +3293,7 @@
       <c r="B27" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="68"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -3305,7 +3305,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="68"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -3317,7 +3317,7 @@
       <c r="B29" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -3329,7 +3329,7 @@
       <c r="B30" s="45">
         <v>1</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -3365,7 +3365,7 @@
       <c r="B33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -3377,7 +3377,7 @@
       <c r="B34" s="45">
         <v>0</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -3389,7 +3389,7 @@
       <c r="B35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -3401,7 +3401,7 @@
       <c r="B36" s="45">
         <v>0</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="10"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -3413,7 +3413,7 @@
       <c r="B37" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="68"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -3425,7 +3425,7 @@
       <c r="B38" s="45">
         <v>0</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="10"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -3497,6 +3497,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C3:C4"/>
@@ -3509,11 +3514,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3572,7 +3572,7 @@
       <c r="B3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3584,7 +3584,7 @@
       <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="32"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -3596,7 +3596,7 @@
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="32"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3608,7 +3608,7 @@
       <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="32"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -3620,7 +3620,7 @@
       <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="32"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3632,7 +3632,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -3644,7 +3644,7 @@
       <c r="B9" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -3656,7 +3656,7 @@
       <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -3668,7 +3668,7 @@
       <c r="B11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="65"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -3680,7 +3680,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="65"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -3716,7 +3716,7 @@
       <c r="B15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="65"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -3728,7 +3728,7 @@
       <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="65"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -3740,7 +3740,7 @@
       <c r="B17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="65"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3752,7 +3752,7 @@
       <c r="B18" s="45">
         <v>0.5</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="65"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -3788,7 +3788,7 @@
       <c r="B21" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -3800,7 +3800,7 @@
       <c r="B22" s="45">
         <v>1</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3836,7 +3836,7 @@
       <c r="B25" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="68"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="12"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -3848,7 +3848,7 @@
       <c r="B26" s="45">
         <v>1</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -3860,7 +3860,7 @@
       <c r="B27" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="68"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -3872,7 +3872,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="68"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -3884,7 +3884,7 @@
       <c r="B29" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -3896,7 +3896,7 @@
       <c r="B30" s="45">
         <v>1</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -3932,7 +3932,7 @@
       <c r="B33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -3944,7 +3944,7 @@
       <c r="B34" s="45">
         <v>1</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -3956,7 +3956,7 @@
       <c r="B35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -3968,7 +3968,7 @@
       <c r="B36" s="45">
         <v>0</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="10"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -3980,7 +3980,7 @@
       <c r="B37" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="68"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -3992,7 +3992,7 @@
       <c r="B38" s="45">
         <v>0</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="10"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -4064,6 +4064,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C3:C4"/>
@@ -4076,11 +4081,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4139,7 +4139,7 @@
       <c r="B3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4151,7 +4151,7 @@
       <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="32"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -4163,7 +4163,7 @@
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="32"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4175,7 +4175,7 @@
       <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="32"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4187,7 +4187,7 @@
       <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="32"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4199,7 +4199,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -4211,7 +4211,7 @@
       <c r="B9" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -4223,7 +4223,7 @@
       <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -4235,7 +4235,7 @@
       <c r="B11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="65"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -4247,7 +4247,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="65"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -4283,7 +4283,7 @@
       <c r="B15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="65"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -4295,7 +4295,7 @@
       <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="65"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -4307,7 +4307,7 @@
       <c r="B17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="65"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -4319,7 +4319,7 @@
       <c r="B18" s="45">
         <v>0.5</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="65"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4355,7 +4355,7 @@
       <c r="B21" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -4367,7 +4367,7 @@
       <c r="B22" s="45">
         <v>1</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -4403,7 +4403,7 @@
       <c r="B25" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="68"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="12"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -4415,7 +4415,7 @@
       <c r="B26" s="45">
         <v>1</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -4427,7 +4427,7 @@
       <c r="B27" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="68"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -4439,7 +4439,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="68"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -4451,7 +4451,7 @@
       <c r="B29" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -4463,7 +4463,7 @@
       <c r="B30" s="45">
         <v>1</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -4499,7 +4499,7 @@
       <c r="B33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -4511,7 +4511,7 @@
       <c r="B34" s="45">
         <v>1</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -4523,7 +4523,7 @@
       <c r="B35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -4535,7 +4535,7 @@
       <c r="B36" s="45">
         <v>0</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="10"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -4547,7 +4547,7 @@
       <c r="B37" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="68"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -4559,7 +4559,7 @@
       <c r="B38" s="45">
         <v>0</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="10"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -4631,6 +4631,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C3:C4"/>
@@ -4643,11 +4648,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4706,7 +4706,7 @@
       <c r="B3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4718,7 +4718,7 @@
       <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="32"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -4730,7 +4730,7 @@
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="32"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4742,7 +4742,7 @@
       <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="32"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4754,7 +4754,7 @@
       <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="32"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4766,7 +4766,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -4778,7 +4778,7 @@
       <c r="B9" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -4790,7 +4790,7 @@
       <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -4802,7 +4802,7 @@
       <c r="B11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="65"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -4814,7 +4814,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="65"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -4850,7 +4850,7 @@
       <c r="B15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="65"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -4862,7 +4862,7 @@
       <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="65"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -4874,7 +4874,7 @@
       <c r="B17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="65"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -4886,7 +4886,7 @@
       <c r="B18" s="45">
         <v>1</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="65"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4922,7 +4922,7 @@
       <c r="B21" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -4934,7 +4934,7 @@
       <c r="B22" s="45">
         <v>1</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -4970,7 +4970,7 @@
       <c r="B25" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="68"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="12"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -4982,7 +4982,7 @@
       <c r="B26" s="45">
         <v>1</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -4994,7 +4994,7 @@
       <c r="B27" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="68"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -5006,7 +5006,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="68"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -5018,7 +5018,7 @@
       <c r="B29" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -5030,7 +5030,7 @@
       <c r="B30" s="45">
         <v>1</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -5066,7 +5066,7 @@
       <c r="B33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -5078,7 +5078,7 @@
       <c r="B34" s="45">
         <v>1</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -5090,7 +5090,7 @@
       <c r="B35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -5102,7 +5102,7 @@
       <c r="B36" s="45">
         <v>0</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="10"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -5114,7 +5114,7 @@
       <c r="B37" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="68"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -5126,7 +5126,7 @@
       <c r="B38" s="45">
         <v>0</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="10"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -5198,6 +5198,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C3:C4"/>
@@ -5210,11 +5215,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5273,7 +5273,7 @@
       <c r="B3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -5285,7 +5285,7 @@
       <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="32"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -5297,7 +5297,7 @@
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="32"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -5309,7 +5309,7 @@
       <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="32"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -5321,7 +5321,7 @@
       <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="32"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -5333,7 +5333,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -5345,7 +5345,7 @@
       <c r="B9" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -5357,7 +5357,7 @@
       <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -5369,7 +5369,7 @@
       <c r="B11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="65"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -5381,7 +5381,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="65"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5417,7 +5417,7 @@
       <c r="B15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="65"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -5429,7 +5429,7 @@
       <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="65"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -5441,7 +5441,7 @@
       <c r="B17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="65"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -5453,7 +5453,7 @@
       <c r="B18" s="45">
         <v>1</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="65"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -5489,7 +5489,7 @@
       <c r="B21" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -5501,7 +5501,7 @@
       <c r="B22" s="45">
         <v>1</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -5537,7 +5537,7 @@
       <c r="B25" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="68"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="12"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -5549,7 +5549,7 @@
       <c r="B26" s="45">
         <v>1</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -5561,7 +5561,7 @@
       <c r="B27" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="68"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -5573,7 +5573,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="68"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -5585,7 +5585,7 @@
       <c r="B29" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -5597,7 +5597,7 @@
       <c r="B30" s="45">
         <v>1</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -5633,7 +5633,7 @@
       <c r="B33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -5645,7 +5645,7 @@
       <c r="B34" s="45">
         <v>0</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -5657,7 +5657,7 @@
       <c r="B35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -5669,7 +5669,7 @@
       <c r="B36" s="45">
         <v>0</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="10"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -5681,7 +5681,7 @@
       <c r="B37" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="68"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -5693,7 +5693,7 @@
       <c r="B38" s="45">
         <v>0.5</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="10"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -5768,6 +5768,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C3:C4"/>
@@ -5780,11 +5785,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5794,9 +5794,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC705C2D-8278-2E4B-8A6E-237F8F029BF8}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A34:C40"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25" defaultRowHeight="40" customHeight="1"/>
@@ -10148,7 +10148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0519FC-3441-E343-AF5D-5F36F764B28C}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B35" sqref="B28:B35"/>
     </sheetView>
@@ -10197,7 +10197,7 @@
       <c r="B3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -10209,7 +10209,7 @@
       <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="32"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -10221,7 +10221,7 @@
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="32"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -10233,7 +10233,7 @@
       <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="32"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -10245,7 +10245,7 @@
       <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="32"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -10257,7 +10257,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -10269,7 +10269,7 @@
       <c r="B9" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -10281,7 +10281,7 @@
       <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -10293,7 +10293,7 @@
       <c r="B11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="65"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -10305,7 +10305,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="65"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -10341,7 +10341,7 @@
       <c r="B15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="65"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -10353,7 +10353,7 @@
       <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="65"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -10365,7 +10365,7 @@
       <c r="B17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="65"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -10377,7 +10377,7 @@
       <c r="B18" s="45">
         <v>1</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="65"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -10413,7 +10413,7 @@
       <c r="B21" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -10425,7 +10425,7 @@
       <c r="B22" s="45">
         <v>1</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -10461,7 +10461,7 @@
       <c r="B25" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="68"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="12"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -10473,7 +10473,7 @@
       <c r="B26" s="45">
         <v>1</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -10485,7 +10485,7 @@
       <c r="B27" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="68"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -10497,7 +10497,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="68"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -10509,7 +10509,7 @@
       <c r="B29" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -10521,7 +10521,7 @@
       <c r="B30" s="45">
         <v>1</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -10557,7 +10557,7 @@
       <c r="B33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -10569,7 +10569,7 @@
       <c r="B34" s="45">
         <v>0</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -10581,7 +10581,7 @@
       <c r="B35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -10593,7 +10593,7 @@
       <c r="B36" s="45">
         <v>0</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="10"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -10605,7 +10605,7 @@
       <c r="B37" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="68"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -10617,7 +10617,7 @@
       <c r="B38" s="45">
         <v>0</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="10"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -10689,11 +10689,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C29:C30"/>
@@ -10701,11 +10701,11 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C15:C16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -10764,7 +10764,7 @@
       <c r="B3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -10776,7 +10776,7 @@
       <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="32"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -10788,7 +10788,7 @@
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="32"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -10800,7 +10800,7 @@
       <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="32"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -10812,7 +10812,7 @@
       <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="32"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -10824,7 +10824,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -10836,7 +10836,7 @@
       <c r="B9" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -10848,7 +10848,7 @@
       <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -10860,7 +10860,7 @@
       <c r="B11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="65"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -10872,7 +10872,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="65"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -10908,7 +10908,7 @@
       <c r="B15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="65"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -10920,7 +10920,7 @@
       <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="65"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -10932,7 +10932,7 @@
       <c r="B17" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="65"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -10944,7 +10944,7 @@
       <c r="B18" s="45">
         <v>1</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="65"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -10980,7 +10980,7 @@
       <c r="B21" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -10992,7 +10992,7 @@
       <c r="B22" s="45">
         <v>1</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -11028,7 +11028,7 @@
       <c r="B25" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="68"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="12"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -11040,7 +11040,7 @@
       <c r="B26" s="45">
         <v>1</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -11052,7 +11052,7 @@
       <c r="B27" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="68"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -11064,7 +11064,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="68"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -11076,7 +11076,7 @@
       <c r="B29" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -11088,7 +11088,7 @@
       <c r="B30" s="45">
         <v>1</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -11124,7 +11124,7 @@
       <c r="B33" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -11136,7 +11136,7 @@
       <c r="B34" s="45">
         <v>1</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -11148,7 +11148,7 @@
       <c r="B35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -11160,7 +11160,7 @@
       <c r="B36" s="45">
         <v>0</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="10"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -11172,7 +11172,7 @@
       <c r="B37" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="68"/>
+      <c r="C37" s="69"/>
       <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -11184,7 +11184,7 @@
       <c r="B38" s="45">
         <v>0</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="10"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -11256,6 +11256,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C3:C4"/>
@@ -11268,11 +11273,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>